<commit_message>
- TL & Modify a bunch, see git log
</commit_message>
<xml_diff>
--- a/tl/P00230.MES.BIN.xlsx
+++ b/tl/P00230.MES.BIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0348EE4-82CC-4D8C-8FF3-B4FD4D55EBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F12C33-2169-401B-A97E-A4FA9666A562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="15780" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="54585" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P00230.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <t>Touya</t>
   </si>
   <si>
-    <t>I started working as a home tutor.</t>
+    <t>I started working as a tutor.</t>
   </si>
   <si>
     <t>3</t>
@@ -65,7 +65,7 @@
     <t>Yuki</t>
   </si>
   <si>
-    <t>Ah, so you got the one you applied for?</t>
+    <t>Ah, so you got the job you applied for?</t>
   </si>
   <si>
     <t>5</t>
@@ -77,25 +77,25 @@
     <t>7</t>
   </si>
   <si>
-    <t>Ah, but don't push yourself too hard.</t>
+    <t>Ah, but don't overdo it and push yourself too hard.</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>It's fine. It's just once a week.</t>
+    <t>It's fine. It's only once a week.</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>Heh, really?</t>
+    <t>Wow, that's it?</t>
   </si>
   <si>
     <t>13</t>
   </si>
   <si>
-    <t>Ah, she's surprised.</t>
+    <t>Ah, she sounds surprised.</t>
   </si>
   <si>
     <t>15</t>
@@ -107,19 +107,19 @@
     <t>17</t>
   </si>
   <si>
-    <t>Plus, I can take days off whenever I want, so there aren't many part-time jobs as easygoing as this one.</t>
+    <t>Plus, I can take days off whenever I want; there aren't many part-time jobs this easygoing.</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>And the student is a test-taker.</t>
+    <t>And I'm teaching an exam student.</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>Touya-kun… really…?</t>
+    <t>Touya-kun… Are you really…?</t>
   </si>
   <si>
     <t>23</t>
@@ -137,88 +137,88 @@
     <t>27</t>
   </si>
   <si>
-    <t>Yuki, it's not as bad as you're making it out to be.</t>
+    <t>Yuki, you don't have to worry so much.</t>
   </si>
   <si>
     <t>29</t>
   </si>
   <si>
-    <t>Even Yuki tells me not to push myself too hard. I wonder if I really do.</t>
+    <t>Even Yuki is telling me not to push myself too hard, huh.</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
-    <t>There are times when I wish I could always be by your side to help…</t>
+    <t>It's just that, Touya-kun… Sometimes you really do overdo it…</t>
   </si>
   <si>
     <t>33</t>
   </si>
   <si>
-    <t>But, Touya-kun… sometimes you really do push yourself…</t>
+    <t>…There are times when I wish I could be with you all the time…</t>
   </si>
   <si>
     <t>35</t>
   </si>
   <si>
-    <t>…There are times when I wish I could always be by your side to help…</t>
+    <t>It's okay. I'm not overdoing it.</t>
   </si>
   <si>
     <t>37</t>
   </si>
   <si>
-    <t>It's fine. I'm not pushing myself.</t>
+    <t>Okay…</t>
   </si>
   <si>
     <t>39</t>
   </si>
   <si>
-    <t>Okay…</t>
+    <t>I get it…</t>
   </si>
   <si>
     <t>41</t>
   </si>
   <si>
-    <t>I understand…</t>
+    <t>Whether it's a lie or the truth,</t>
   </si>
   <si>
     <t>43</t>
   </si>
   <si>
-    <t>Whether it's an obvious lie or the truth,</t>
+    <t>there are times when it's better to say things like this.</t>
   </si>
   <si>
     <t>45</t>
   </si>
   <si>
-    <t>there are times when it's better to just say something like this.</t>
+    <t>I promise. I won't push myself to hard. I swear it.</t>
   </si>
   <si>
     <t>47</t>
   </si>
   <si>
-    <t>I promise. I won't push myself. Absolutely.</t>
+    <t>Okay.</t>
   </si>
   <si>
     <t>49</t>
   </si>
   <si>
-    <t>Okay.</t>
+    <t>Do you feel relieved?</t>
   </si>
   <si>
     <t>51</t>
   </si>
   <si>
-    <t>Do you feel relieved?</t>
-  </si>
-  <si>
     <t>53</t>
   </si>
   <si>
+    <t>For example, there are times when just saying something like this is enough.</t>
+  </si>
+  <si>
     <t>55</t>
   </si>
   <si>
-    <t>For example, there are times when it's enough to just say something like this.</t>
+    <t>Even if it's meaningless, there are times when words alone are desired.</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1502,7 @@
         <v>9</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>9</v>
@@ -1519,22 +1519,22 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>9</v>

</xml_diff>